<commit_message>
Fix multiple genes in alteration table
</commit_message>
<xml_diff>
--- a/project-2/Genes-CDS.xlsx
+++ b/project-2/Genes-CDS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Archivio\Scuola\Uni\LM\2\Bioinfo\p-1\project-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEC5FF8-874B-42E2-B4DF-EB5DFC0F08CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5D3443-7296-4BF8-9790-8D395CFFCE8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21852" yWindow="3372" windowWidth="22260" windowHeight="17988" activeTab="1" xr2:uid="{9F754CF9-FD38-434B-846C-C2DEE7A781AF}"/>
+    <workbookView xWindow="23004" yWindow="6168" windowWidth="22260" windowHeight="17988" activeTab="1" xr2:uid="{9F754CF9-FD38-434B-846C-C2DEE7A781AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Geni" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Gene ID</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>ORF10</t>
+  </si>
+  <si>
+    <t>join_at</t>
   </si>
 </sst>
 </file>
@@ -153,7 +156,25 @@
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -249,7 +270,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C86F85F3-EB22-435A-971A-3D91B1DDB56D}" name="Tabella1" displayName="Tabella1" ref="A1:C12" totalsRowShown="0">
   <autoFilter ref="A1:C12" xr:uid="{734EB690-F25E-42E9-96BE-5EC35155F76D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{073292FC-277F-4451-8FEE-C0A5D941A17B}" name="Gene ID" dataDxfId="5" dataCellStyle="Collegamento ipertestuale"/>
+    <tableColumn id="1" xr3:uid="{073292FC-277F-4451-8FEE-C0A5D941A17B}" name="Gene ID" dataDxfId="6" dataCellStyle="Collegamento ipertestuale"/>
     <tableColumn id="2" xr3:uid="{577ACA37-B974-4E26-918D-B2298D4AFA03}" name="Start"/>
     <tableColumn id="3" xr3:uid="{7102894A-3A47-4726-9195-D5E371A419D0}" name="End"/>
   </tableColumns>
@@ -258,13 +279,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0261EE6C-11B5-4E45-8B5D-3C96498787EE}" name="Tabella2" displayName="Tabella2" ref="A1:D12" totalsRowShown="0" dataDxfId="4">
-  <autoFilter ref="A1:D12" xr:uid="{1F041A3E-6C3C-467F-8B66-D18E6EB2A738}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0088FC1F-8151-4651-B954-7C5465E13E45}" name="gene" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{BFE7175F-5FD5-4442-AB3A-DF930186CBA5}" name="GeneID" dataDxfId="2" dataCellStyle="Collegamento ipertestuale"/>
-    <tableColumn id="3" xr3:uid="{07B8D2AE-98E5-4CBE-A538-B9D5FDBD4795}" name="from" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{878F625A-390E-4029-9EA4-FB00849E70C1}" name="to" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0261EE6C-11B5-4E45-8B5D-3C96498787EE}" name="Tabella2" displayName="Tabella2" ref="A1:E13" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E13" xr:uid="{1F041A3E-6C3C-467F-8B66-D18E6EB2A738}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{0088FC1F-8151-4651-B954-7C5465E13E45}" name="gene" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{BFE7175F-5FD5-4442-AB3A-DF930186CBA5}" name="GeneID" dataDxfId="3" dataCellStyle="Collegamento ipertestuale"/>
+    <tableColumn id="3" xr3:uid="{07B8D2AE-98E5-4CBE-A538-B9D5FDBD4795}" name="from" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{878F625A-390E-4029-9EA4-FB00849E70C1}" name="to" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{80703E01-0213-4D56-BDCA-D580BF39A980}" name="join_at" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -734,10 +756,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3671BA5D-5657-41F0-9937-267A1BD6B181}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -758,6 +780,9 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6">
@@ -773,6 +798,7 @@
       <c r="D2" s="2">
         <v>13483</v>
       </c>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
@@ -787,6 +813,7 @@
       <c r="D3" s="2">
         <v>25384</v>
       </c>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
@@ -801,6 +828,7 @@
       <c r="D4" s="2">
         <v>26220</v>
       </c>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
@@ -815,6 +843,7 @@
       <c r="D5" s="2">
         <v>26472</v>
       </c>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
@@ -829,6 +858,7 @@
       <c r="D6" s="2">
         <v>27191</v>
       </c>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
@@ -843,6 +873,7 @@
       <c r="D7" s="2">
         <v>27387</v>
       </c>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
@@ -857,6 +888,7 @@
       <c r="D8" s="2">
         <v>27759</v>
       </c>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
@@ -871,6 +903,7 @@
       <c r="D9" s="2">
         <v>27887</v>
       </c>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="2" t="s">
@@ -885,6 +918,7 @@
       <c r="D10" s="2">
         <v>28259</v>
       </c>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
@@ -899,6 +933,7 @@
       <c r="D11" s="2">
         <v>29533</v>
       </c>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
@@ -912,6 +947,24 @@
       </c>
       <c r="D12" s="2">
         <v>29674</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="3">
+        <v>43740578</v>
+      </c>
+      <c r="C13" s="2">
+        <v>266</v>
+      </c>
+      <c r="D13" s="2">
+        <v>21555</v>
+      </c>
+      <c r="E13" s="2">
+        <v>13468</v>
       </c>
     </row>
   </sheetData>

</xml_diff>